<commit_message>
split reference managers off into excel_reference_managers.py and added link hiding capability
</commit_message>
<xml_diff>
--- a/Python/tests/test_out_xlsx.xlsx
+++ b/Python/tests/test_out_xlsx.xlsx
@@ -1,13 +1,38 @@
+
+<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
+  <workbookProtection/>
+  <bookViews>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+  </sheets>
+  <definedNames/>
+  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+</workbook>
+</file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color theme="10"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -19,7 +44,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -27,15 +52,27 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="0"/>
   </cellStyles>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
@@ -390,4 +427,69 @@
   <a:objectDefaults/>
   <a:extraClrSchemeLst/>
 </a:theme>
+</file>
+
+<file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="B2:D4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="2">
+      <c r="C2" s="1" t="inlineStr">
+        <is>
+          <t>name</t>
+        </is>
+      </c>
+      <c r="D2" s="1" t="inlineStr">
+        <is>
+          <t>url</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="B3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Google</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>LINK</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Stackoverflow</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>LINK</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D3" r:id="rId1"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="D4" r:id="rId2"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>